<commit_message>
MAJOR CHANGES: restructure repo for versioning
- restructures the repo with two folders for v1.0 and v2.0
- changes the IRI for v2.0 to w3id.org/dpv/v2.0 as prefix
- copied media folder into v2.0 to avoid breaking diagram urls - in the
  future, the unused diagrams should be removed from it
- primer, guides, examples, and ucr are kept in root folder and not
  moved into versioned folders
</commit_message>
<xml_diff>
--- a/code/vocab_csv/namespaces.xlsx
+++ b/code/vocab_csv/namespaces.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="249">
   <si>
     <t>preffix</t>
   </si>
@@ -259,70 +259,73 @@
     <t>AI Technology concepts extending DPV</t>
   </si>
   <si>
-    <t>https://w3id.org/dpv/v2/risk#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/examples#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/rights#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/use-cases#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/nace#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/eu/gdpr#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/pd#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/tech#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/rights/eu#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/eu/dga#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/eu/aiact#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/eu/nis2#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/loc#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/eu#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/de#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/ie#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/gb#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/us#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/legal/in#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/justifications#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2/ai#</t>
+    <t>https://w3id.org/dpv/v2.0#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/risk#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/examples#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/rights#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/use-cases#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/nace#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/eu/gdpr#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/pd#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/tech#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/rights/eu#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/eu/dga#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/eu/aiact#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/eu/nis2#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/loc#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/eu#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/de#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/ie#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/gb#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/us#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/legal/in#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/justifications#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/v2.0/ai#</t>
   </si>
   <si>
     <t>dct</t>
@@ -1841,8 +1844,8 @@
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>9</v>
+      <c r="B2" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
@@ -1862,7 +1865,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>15</v>
@@ -1882,7 +1885,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>19</v>
@@ -1899,7 +1902,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>22</v>
@@ -1916,7 +1919,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>25</v>
@@ -1933,7 +1936,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>28</v>
@@ -1953,7 +1956,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>31</v>
@@ -1973,7 +1976,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>34</v>
@@ -1993,7 +1996,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>37</v>
@@ -2013,7 +2016,7 @@
         <v>38</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>40</v>
@@ -2033,7 +2036,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>41</v>
@@ -2053,7 +2056,7 @@
         <v>42</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>44</v>
@@ -2073,7 +2076,7 @@
         <v>45</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>47</v>
@@ -2093,7 +2096,7 @@
         <v>48</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>50</v>
@@ -2113,7 +2116,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>53</v>
@@ -2133,7 +2136,7 @@
         <v>54</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>56</v>
@@ -2153,7 +2156,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>59</v>
@@ -2173,7 +2176,7 @@
         <v>60</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>62</v>
@@ -2193,7 +2196,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>65</v>
@@ -2210,7 +2213,7 @@
         <v>66</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>68</v>
@@ -2227,7 +2230,7 @@
         <v>69</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>71</v>
@@ -2244,7 +2247,7 @@
         <v>72</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>74</v>
@@ -2261,7 +2264,7 @@
         <v>75</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>77</v>
@@ -2278,7 +2281,7 @@
         <v>78</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>80</v>
@@ -2365,13 +2368,13 @@
     </row>
     <row r="2">
       <c r="A2" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -2395,13 +2398,13 @@
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
@@ -2425,13 +2428,13 @@
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
@@ -2455,13 +2458,13 @@
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
@@ -2485,13 +2488,13 @@
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
@@ -2515,13 +2518,13 @@
     </row>
     <row r="7">
       <c r="A7" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -2545,10 +2548,10 @@
     </row>
     <row r="8">
       <c r="A8" s="19" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C8" s="25" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
@@ -2576,13 +2579,13 @@
     </row>
     <row r="9">
       <c r="A9" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
@@ -2606,13 +2609,13 @@
     </row>
     <row r="10">
       <c r="A10" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
@@ -2636,13 +2639,13 @@
     </row>
     <row r="11">
       <c r="A11" s="27" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
@@ -2666,13 +2669,13 @@
     </row>
     <row r="12">
       <c r="A12" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
@@ -2696,13 +2699,13 @@
     </row>
     <row r="13">
       <c r="A13" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -2726,13 +2729,13 @@
     </row>
     <row r="14">
       <c r="A14" s="27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -2756,134 +2759,134 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2930,10 +2933,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>28</v>
@@ -2950,13 +2953,13 @@
     </row>
     <row r="2">
       <c r="A2" s="31" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -2970,13 +2973,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -2990,13 +2993,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -3005,18 +3008,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -3025,34 +3028,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -3066,13 +3069,13 @@
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -3086,13 +3089,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -3106,13 +3109,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -3121,18 +3124,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -3141,18 +3144,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -3161,18 +3164,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -3186,13 +3189,13 @@
     </row>
     <row r="14">
       <c r="A14" s="31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -3206,13 +3209,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -3226,13 +3229,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -3241,18 +3244,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -3261,18 +3264,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -3281,18 +3284,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -3306,13 +3309,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -3326,13 +3329,13 @@
     </row>
     <row r="21">
       <c r="A21" s="32" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B21" s="33" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D21" s="34">
         <v>44734.0</v>
@@ -3362,13 +3365,13 @@
     </row>
     <row r="22">
       <c r="A22" s="32" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D22" s="34">
         <v>44734.0</v>
@@ -3398,13 +3401,13 @@
     </row>
     <row r="23">
       <c r="A23" s="32" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D23" s="34">
         <v>44734.0</v>
@@ -3434,13 +3437,13 @@
     </row>
     <row r="24">
       <c r="A24" s="32" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D24" s="34">
         <v>45189.0</v>

</xml_diff>

<commit_message>
changes version namespace, IRI, folders as vX to X
- see #45 https://github.com/w3c/dpv/issues/45#issuecomment-2184828519
- DPV versions were expressed as "v2.0" and this string was used in the
  IRIs, folder structures, etc. Following the best practice
  recommendation of not starting versions with letters, the prefix 'v'
  has been dropped and all RDF, HTML, and other resources have been
  regenerated
</commit_message>
<xml_diff>
--- a/code/vocab_csv/namespaces.xlsx
+++ b/code/vocab_csv/namespaces.xlsx
@@ -259,73 +259,73 @@
     <t>AI Technology concepts extending DPV</t>
   </si>
   <si>
-    <t>https://w3id.org/dpv/v2.0#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/risk#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/examples#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/rights#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/use-cases#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/nace#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/eu/gdpr#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/pd#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/tech#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/rights/eu#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/eu/dga#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/eu/aiact#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/eu/nis2#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/loc#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/eu#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/de#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/ie#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/gb#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/us#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/legal/in#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/justifications#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/v2.0/ai#</t>
+    <t>https://w3id.org/dpv/2.0#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/risk#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/examples#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/rights#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/use-cases#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/nace#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/eu/gdpr#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/pd#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/tech#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/rights/eu#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/eu/dga#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/eu/aiact#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/eu/nis2#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/loc#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/eu#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/de#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/ie#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/gb#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/us#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/legal/in#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/justifications#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/2.0/ai#</t>
   </si>
   <si>
     <t>dct</t>

</xml_diff>

<commit_message>
adds legal extensions for EU/EEA member states
- adds extensions under `/legal` for the following EU/EEA member states:
  AT, BE, BG, CY, CZ, DK, EE, ES, FI, FR, GB, GR, HR, HU,
  IS, IT, LI, LT, LU, LV, MT, NL, NO, PL, PT, RO, SE, SI, SK,
  which use the ISO 3166-2 codes
- the following extensions already existed in 2.0: IE, IN, DE, US, EU
- each jurisdiction only has the DPA defined, and no laws are defined at
  the moment
- #48 should be used to discuss this - the missing laws and other info
  requires volunteers to collect the data (the work is quite simple)
- Spain (ES) has 3 autonomous regions who have DPAs, whose data is
  present in the spreadsheets but has not been included in this release
  as their jurisdictions utilise regions which are not currently
  represented in LOC
- #179 tracks the addition of ISO 3166-2 subdivisions which are needed
  to add ES data as above
</commit_message>
<xml_diff>
--- a/code/vocab_csv/namespaces.xlsx
+++ b/code/vocab_csv/namespaces.xlsx
@@ -4,9 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Namespaces" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Namespaces-v2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Namespaces_Other" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Namespaces_old" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Namespaces_Other" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Namespaces_old" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="313">
   <si>
     <t>preffix</t>
   </si>
@@ -187,22 +186,166 @@
     <t>Location concepts extended DPV</t>
   </si>
   <si>
+    <t>justifications</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/justifications#</t>
+  </si>
+  <si>
+    <t>Justifications for use with DPV concepts</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/ai#</t>
+  </si>
+  <si>
+    <t>AI Technology concepts extending DPV</t>
+  </si>
+  <si>
+    <t>legal-at</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/at#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for AT</t>
+  </si>
+  <si>
+    <t>legal-be</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/be#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for BE</t>
+  </si>
+  <si>
+    <t>legal-bg</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/bg#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for BG</t>
+  </si>
+  <si>
+    <t>legal-cy</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/cy#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for CY</t>
+  </si>
+  <si>
+    <t>legal-cz</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/cz#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for CZ</t>
+  </si>
+  <si>
+    <t>legal-de</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/de#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for DE</t>
+  </si>
+  <si>
+    <t>legal-dk</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/dk#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for DK</t>
+  </si>
+  <si>
+    <t>legal-ee</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/ee#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for EE</t>
+  </si>
+  <si>
+    <t>legal-es</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/es#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for ES</t>
+  </si>
+  <si>
     <t>legal-eu</t>
   </si>
   <si>
     <t>https://w3id.org/dpv/legal/eu#</t>
   </si>
   <si>
-    <t>Laws, Authorities, and other Legal concepts for European Union (EU) as Jurisdiction</t>
-  </si>
-  <si>
-    <t>legal-de</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/legal/de#</t>
-  </si>
-  <si>
-    <t>Laws, Authorities, and other Legal concepts for Germany (DE) as Jurisdiction</t>
+    <t>Laws and Authorities for EU</t>
+  </si>
+  <si>
+    <t>legal-fi</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/fi#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for FI</t>
+  </si>
+  <si>
+    <t>legal-fr</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/fr#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for FR</t>
+  </si>
+  <si>
+    <t>legal-gb</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/gb#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for GB</t>
+  </si>
+  <si>
+    <t>legal-gr</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/gr#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for GR</t>
+  </si>
+  <si>
+    <t>legal-hr</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/hr#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for HR</t>
+  </si>
+  <si>
+    <t>legal-hu</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/hu#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for HU</t>
   </si>
   <si>
     <t>legal-ie</t>
@@ -211,16 +354,151 @@
     <t>https://w3id.org/dpv/legal/ie#</t>
   </si>
   <si>
-    <t>Laws, Authorities, and other Legal concepts for Ireland (IE) as Jurisdiction</t>
-  </si>
-  <si>
-    <t>legal-gb</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/legal/gb#</t>
-  </si>
-  <si>
-    <t>Laws, Authorities, and other Legal concepts for United Kingdom (GB) as Jurisdiction</t>
+    <t>Laws and Authorities for IE</t>
+  </si>
+  <si>
+    <t>legal-in</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/in#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for IN</t>
+  </si>
+  <si>
+    <t>legal-is</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/is#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for IS</t>
+  </si>
+  <si>
+    <t>legal-it</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/it#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for IT</t>
+  </si>
+  <si>
+    <t>legal-li</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/li#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for LI</t>
+  </si>
+  <si>
+    <t>legal-lt</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/lt#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for LT</t>
+  </si>
+  <si>
+    <t>legal-lu</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/lu#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for LU</t>
+  </si>
+  <si>
+    <t>legal-lv</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/lv#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for LV</t>
+  </si>
+  <si>
+    <t>legal-mt</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/mt#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for MT</t>
+  </si>
+  <si>
+    <t>legal-nl</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/nl#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for NL</t>
+  </si>
+  <si>
+    <t>legal-no</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/no#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for NO</t>
+  </si>
+  <si>
+    <t>legal-pl</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/pl#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for PL</t>
+  </si>
+  <si>
+    <t>legal-pt</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/pt#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for PT</t>
+  </si>
+  <si>
+    <t>legal-ro</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/ro#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for RO</t>
+  </si>
+  <si>
+    <t>legal-se</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/se#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for SE</t>
+  </si>
+  <si>
+    <t>legal-si</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/si#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for SI</t>
+  </si>
+  <si>
+    <t>legal-sk</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/sk#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for SK</t>
   </si>
   <si>
     <t>legal-us</t>
@@ -229,103 +507,7 @@
     <t>https://w3id.org/dpv/legal/us#</t>
   </si>
   <si>
-    <t>Laws, Authorities, and other Legal concepts for United States of America (USA) as Jurisdiction</t>
-  </si>
-  <si>
-    <t>legal-in</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/legal/in#</t>
-  </si>
-  <si>
-    <t>Laws, Authorities, and other Legal concepts for India (IE) as Jurisdiction</t>
-  </si>
-  <si>
-    <t>justifications</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/justifications#</t>
-  </si>
-  <si>
-    <t>Justifications for use with DPV concepts</t>
-  </si>
-  <si>
-    <t>ai</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/ai#</t>
-  </si>
-  <si>
-    <t>AI Technology concepts extending DPV</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/risk#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/examples#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/rights#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/use-cases#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/nace#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/eu/gdpr#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/pd#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/tech#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/rights/eu#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/eu/dga#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/eu/aiact#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/eu/nis2#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/loc#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/eu#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/de#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/ie#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/gb#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/us#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/legal/in#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/justifications#</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/2.0/ai#</t>
+    <t>Laws and Authorities for US</t>
   </si>
   <si>
     <t>dct</t>
@@ -776,10 +958,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -843,10 +1026,15 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Aptos Narrow&quot;"/>
+    </font>
+    <font>
       <u/>
-      <sz val="8.0"/>
-      <color rgb="FF0000FF"/>
-      <name val="&quot;Arial&quot;"/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
       <u/>
@@ -958,7 +1146,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1014,18 +1202,21 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1041,28 +1232,31 @@
     <xf borderId="0" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1082,10 +1276,6 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1635,144 +1825,614 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D18" s="8">
         <v>45455.0</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="E18" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="6" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="8">
         <v>45455.0</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="E19" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E20" s="16" t="s">
+      <c r="D20" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E21" s="16" t="s">
+      <c r="D21" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E22" s="16" t="s">
+      <c r="D22" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E23" s="16" t="s">
+      <c r="D23" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="D25" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="20">
+        <v>45330.0</v>
+      </c>
+      <c r="E53" s="18" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1804,8 +2464,36 @@
     <hyperlink r:id="rId24" ref="B23"/>
     <hyperlink r:id="rId25" ref="B24"/>
     <hyperlink r:id="rId26" ref="B25"/>
+    <hyperlink r:id="rId27" ref="B26"/>
+    <hyperlink r:id="rId28" ref="B27"/>
+    <hyperlink r:id="rId29" ref="B28"/>
+    <hyperlink r:id="rId30" ref="B29"/>
+    <hyperlink r:id="rId31" ref="B30"/>
+    <hyperlink r:id="rId32" ref="B31"/>
+    <hyperlink r:id="rId33" ref="B32"/>
+    <hyperlink r:id="rId34" ref="B33"/>
+    <hyperlink r:id="rId35" ref="B34"/>
+    <hyperlink r:id="rId36" ref="B35"/>
+    <hyperlink r:id="rId37" ref="B36"/>
+    <hyperlink r:id="rId38" ref="B37"/>
+    <hyperlink r:id="rId39" ref="B38"/>
+    <hyperlink r:id="rId40" ref="B39"/>
+    <hyperlink r:id="rId41" ref="B40"/>
+    <hyperlink r:id="rId42" ref="B41"/>
+    <hyperlink r:id="rId43" ref="B42"/>
+    <hyperlink r:id="rId44" ref="B43"/>
+    <hyperlink r:id="rId45" ref="B44"/>
+    <hyperlink r:id="rId46" ref="B45"/>
+    <hyperlink r:id="rId47" ref="B46"/>
+    <hyperlink r:id="rId48" ref="B47"/>
+    <hyperlink r:id="rId49" ref="B48"/>
+    <hyperlink r:id="rId50" ref="B49"/>
+    <hyperlink r:id="rId51" ref="B50"/>
+    <hyperlink r:id="rId52" ref="B51"/>
+    <hyperlink r:id="rId53" ref="B52"/>
+    <hyperlink r:id="rId54" ref="B53"/>
   </hyperlinks>
-  <drawing r:id="rId27"/>
+  <drawing r:id="rId55"/>
 </worksheet>
 </file>
 
@@ -1850,1063 +2538,537 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A3" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="A4" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="A5" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="A7" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="A8" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="27" t="str">
+        <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
+        <v>SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
     </row>
     <row r="9">
-      <c r="A9" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="A9" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="A11" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
     </row>
     <row r="12">
-      <c r="A12" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="A12" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
     </row>
     <row r="13">
-      <c r="A13" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="A13" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
     </row>
     <row r="14">
-      <c r="A14" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="A14" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
     </row>
     <row r="15">
-      <c r="A15" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="A15" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="A16" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="A17" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="A18" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="A19" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>11</v>
+      <c r="A20" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>11</v>
+      <c r="A21" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>11</v>
+      <c r="A22" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>11</v>
+      <c r="A23" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>11</v>
+      <c r="A24" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>103</v>
+        <v>231</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="8">
-        <v>45455.0</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="H2"/>
-    <hyperlink r:id="rId3" ref="B3"/>
-    <hyperlink r:id="rId4" ref="H3"/>
-    <hyperlink r:id="rId5" ref="B4"/>
-    <hyperlink r:id="rId6" ref="B5"/>
-    <hyperlink r:id="rId7" ref="B6"/>
-    <hyperlink r:id="rId8" ref="B7"/>
-    <hyperlink r:id="rId9" ref="B8"/>
-    <hyperlink r:id="rId10" ref="B9"/>
-    <hyperlink r:id="rId11" ref="B10"/>
-    <hyperlink r:id="rId12" ref="B11"/>
-    <hyperlink r:id="rId13" ref="B12"/>
-    <hyperlink r:id="rId14" ref="B13"/>
-    <hyperlink r:id="rId15" ref="B14"/>
-    <hyperlink r:id="rId16" ref="B15"/>
-    <hyperlink r:id="rId17" ref="B16"/>
-    <hyperlink r:id="rId18" ref="B17"/>
-    <hyperlink r:id="rId19" ref="B18"/>
-    <hyperlink r:id="rId20" ref="B19"/>
-    <hyperlink r:id="rId21" ref="B20"/>
-    <hyperlink r:id="rId22" ref="B21"/>
-    <hyperlink r:id="rId23" ref="B22"/>
-    <hyperlink r:id="rId24" ref="B23"/>
-    <hyperlink r:id="rId25" ref="B24"/>
-    <hyperlink r:id="rId26" ref="B25"/>
-  </hyperlinks>
-  <drawing r:id="rId27"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="36.38"/>
-    <col customWidth="1" min="3" max="3" width="77.0"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="25" t="str">
-        <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
-        <v>SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>172</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>173</v>
+        <v>234</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>174</v>
+        <v>235</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>175</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>176</v>
+        <v>237</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>177</v>
+        <v>238</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>178</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2942,7 +3104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2953,13 +3115,13 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
-        <v>179</v>
+      <c r="A1" s="31" t="s">
+        <v>240</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="8">
@@ -2973,14 +3135,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="31" t="s">
-        <v>181</v>
+      <c r="A2" s="33" t="s">
+        <v>242</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>183</v>
+        <v>243</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>244</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -2994,13 +3156,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>184</v>
+        <v>245</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>185</v>
+        <v>246</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>186</v>
+        <v>247</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -3014,13 +3176,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>187</v>
+        <v>248</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>188</v>
+        <v>249</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>189</v>
+        <v>250</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -3029,18 +3191,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>190</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>191</v>
+        <v>252</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>192</v>
+        <v>253</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>193</v>
+        <v>254</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -3049,34 +3211,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>194</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>195</v>
+        <v>256</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>196</v>
+        <v>257</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>197</v>
+        <v>258</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>198</v>
+        <v>259</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>199</v>
+        <v>260</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>200</v>
+        <v>261</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>201</v>
+        <v>262</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -3089,14 +3251,14 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="31" t="s">
-        <v>202</v>
+      <c r="A8" s="33" t="s">
+        <v>263</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>204</v>
+        <v>264</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>265</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -3110,13 +3272,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>205</v>
+        <v>266</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>206</v>
+        <v>267</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>207</v>
+        <v>268</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -3130,13 +3292,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>208</v>
+        <v>269</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>209</v>
+        <v>270</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>210</v>
+        <v>271</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -3145,18 +3307,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>190</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>213</v>
+        <v>274</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -3165,18 +3327,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>194</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>214</v>
+        <v>275</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>215</v>
+        <v>276</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>216</v>
+        <v>277</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -3185,18 +3347,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>194</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>217</v>
+        <v>278</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>218</v>
+        <v>279</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>219</v>
+        <v>280</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -3209,14 +3371,14 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="31" t="s">
-        <v>220</v>
+      <c r="A14" s="33" t="s">
+        <v>281</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>222</v>
+        <v>282</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>283</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -3230,13 +3392,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>224</v>
+        <v>285</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>225</v>
+        <v>286</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -3250,13 +3412,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>226</v>
+        <v>287</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>227</v>
+        <v>288</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>228</v>
+        <v>289</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -3265,18 +3427,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>190</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>230</v>
+        <v>291</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>231</v>
+        <v>292</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -3285,18 +3447,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>194</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>232</v>
+        <v>293</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>233</v>
+        <v>294</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>234</v>
+        <v>295</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -3305,18 +3467,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>194</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>235</v>
+        <v>296</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>236</v>
+        <v>297</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>237</v>
+        <v>298</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -3330,13 +3492,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>238</v>
+        <v>299</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>239</v>
+        <v>300</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>240</v>
+        <v>301</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -3349,146 +3511,146 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="B21" s="33" t="s">
+      <c r="A21" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="B21" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="D21" s="34">
+      <c r="C21" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="D21" s="36">
         <v>44734.0</v>
       </c>
-      <c r="E21" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="35" t="s">
+      <c r="E21" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="32"/>
-      <c r="V21" s="32"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="34"/>
+      <c r="U21" s="34"/>
+      <c r="V21" s="34"/>
     </row>
     <row r="22">
-      <c r="A22" s="32" t="s">
-        <v>243</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>245</v>
-      </c>
-      <c r="D22" s="34">
+      <c r="A22" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="D22" s="36">
         <v>44734.0</v>
       </c>
-      <c r="E22" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="35" t="s">
+      <c r="E22" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="32"/>
-      <c r="S22" s="32"/>
-      <c r="T22" s="32"/>
-      <c r="U22" s="32"/>
-      <c r="V22" s="32"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="34"/>
+      <c r="T22" s="34"/>
+      <c r="U22" s="34"/>
+      <c r="V22" s="34"/>
     </row>
     <row r="23">
-      <c r="A23" s="32" t="s">
-        <v>246</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>247</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>248</v>
-      </c>
-      <c r="D23" s="34">
+      <c r="A23" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="D23" s="36">
         <v>44734.0</v>
       </c>
-      <c r="E23" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="35" t="s">
+      <c r="E23" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
-      <c r="Q23" s="32"/>
-      <c r="R23" s="32"/>
-      <c r="S23" s="32"/>
-      <c r="T23" s="32"/>
-      <c r="U23" s="32"/>
-      <c r="V23" s="32"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="34"/>
+      <c r="T23" s="34"/>
+      <c r="U23" s="34"/>
+      <c r="V23" s="34"/>
     </row>
     <row r="24">
-      <c r="A24" s="32" t="s">
-        <v>249</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>250</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>251</v>
-      </c>
-      <c r="D24" s="34">
+      <c r="A24" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>311</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="D24" s="36">
         <v>45189.0</v>
       </c>
-      <c r="E24" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="32"/>
+      <c r="E24" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="34"/>
+      <c r="T24" s="34"/>
+      <c r="U24" s="34"/>
+      <c r="V24" s="34"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
adds SECTOR extension with Purposes module
- adds SECTOR extension at path /sector under 2.1-dev
- SECTOR has namespace w3id.org/dpv/sector and prefix sector
- SECTOR has purpose taxonomy added
- SECTOR status is set to draft extension
</commit_message>
<xml_diff>
--- a/code/vocab_csv/namespaces.xlsx
+++ b/code/vocab_csv/namespaces.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="319">
   <si>
     <t>preffix</t>
   </si>
@@ -177,6 +177,15 @@
     <t>EU-NIS2 concepts extended DPV</t>
   </si>
   <si>
+    <t>eu-ehds</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/eu/ehds#</t>
+  </si>
+  <si>
+    <t>EU-EHDS concepts extended DPV</t>
+  </si>
+  <si>
     <t>loc</t>
   </si>
   <si>
@@ -202,6 +211,15 @@
   </si>
   <si>
     <t>AI Technology concepts extending DPV</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/sector#</t>
+  </si>
+  <si>
+    <t>Sector-specific concepts extending DPV</t>
   </si>
   <si>
     <t>legal-at</t>
@@ -962,7 +980,7 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1023,6 +1041,11 @@
       <u/>
       <sz val="8.0"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -1146,7 +1169,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1204,22 +1227,25 @@
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1235,28 +1261,31 @@
     <xf borderId="0" fillId="3" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1805,17 +1834,17 @@
       <c r="H16" s="14"/>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="16" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="8">
-        <v>45455.0</v>
+        <v>45627.0</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>11</v>
@@ -1825,21 +1854,24 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D18" s="8">
         <v>45455.0</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="E18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
@@ -1859,19 +1891,19 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="20">
-        <v>45330.0</v>
-      </c>
-      <c r="E20" s="18" t="s">
+      <c r="D20" s="8">
+        <v>45455.0</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1879,560 +1911,594 @@
       <c r="A21" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="19">
+        <v>45627.0</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="20">
+      <c r="E22" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="20">
+      <c r="E23" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E23" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="20">
+      <c r="E24" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="20">
+      <c r="E25" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="20">
+      <c r="E26" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="20">
+      <c r="E27" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="20">
+      <c r="E28" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E28" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="20">
+      <c r="E29" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E29" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="20">
+      <c r="E30" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E30" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="20">
+      <c r="E31" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" s="20">
+      <c r="E32" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="20">
+      <c r="E33" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="20">
+      <c r="E34" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="20">
+      <c r="E35" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="20">
+      <c r="E36" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E36" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" s="20">
+      <c r="E37" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E37" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="20">
+      <c r="E38" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E38" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D39" s="20">
+      <c r="E39" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E39" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="D40" s="20">
+      <c r="E40" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E40" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D41" s="20">
+      <c r="E41" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E41" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="D42" s="20">
+      <c r="E42" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E42" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="20">
+      <c r="E43" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E43" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D44" s="20">
+      <c r="E44" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E44" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" s="20">
+      <c r="E45" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E45" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="D46" s="20">
+      <c r="E46" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E46" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="20">
+      <c r="E47" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E47" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D48" s="20">
+      <c r="E48" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E48" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="D49" s="20">
+      <c r="E49" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E49" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="D50" s="20">
+      <c r="E50" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E50" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D51" s="20">
+      <c r="E51" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E51" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="D52" s="20">
+      <c r="E52" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E52" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="D53" s="20">
+      <c r="E53" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" s="22">
         <v>45330.0</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E54" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D55" s="22">
+        <v>45330.0</v>
+      </c>
+      <c r="E55" s="20" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2492,8 +2558,10 @@
     <hyperlink r:id="rId52" ref="B51"/>
     <hyperlink r:id="rId53" ref="B52"/>
     <hyperlink r:id="rId54" ref="B53"/>
+    <hyperlink r:id="rId55" ref="B54"/>
+    <hyperlink r:id="rId56" ref="B55"/>
   </hyperlinks>
-  <drawing r:id="rId55"/>
+  <drawing r:id="rId57"/>
 </worksheet>
 </file>
 
@@ -2538,537 +2606,537 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
+      <c r="A2" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
     </row>
     <row r="3">
-      <c r="A3" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
+      <c r="A3" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
     </row>
     <row r="4">
-      <c r="A4" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
+      <c r="A4" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
     </row>
     <row r="5">
-      <c r="A5" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
+      <c r="A5" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
     </row>
     <row r="6">
-      <c r="A6" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
+      <c r="A6" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
     </row>
     <row r="7">
-      <c r="A7" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
+      <c r="A7" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
     </row>
     <row r="8">
-      <c r="A8" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C8" s="27" t="str">
+      <c r="A8" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="29" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
         <v>SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
     </row>
     <row r="9">
-      <c r="A9" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
+      <c r="A9" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
     </row>
     <row r="10">
-      <c r="A10" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
+      <c r="A10" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
     </row>
     <row r="11">
-      <c r="A11" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
+      <c r="A11" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
     </row>
     <row r="12">
-      <c r="A12" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
+      <c r="A12" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
     </row>
     <row r="13">
-      <c r="A13" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
+      <c r="A13" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
     </row>
     <row r="14">
-      <c r="A14" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
+      <c r="A14" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>229</v>
+        <v>234</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>235</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3115,13 +3183,13 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="s">
-        <v>240</v>
+      <c r="A1" s="33" t="s">
+        <v>246</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="C1" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="8">
@@ -3135,14 +3203,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="33" t="s">
-        <v>242</v>
+      <c r="A2" s="35" t="s">
+        <v>248</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>244</v>
+        <v>249</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>250</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -3156,13 +3224,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -3176,13 +3244,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -3191,18 +3259,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -3211,34 +3279,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -3251,14 +3319,14 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="33" t="s">
-        <v>263</v>
+      <c r="A8" s="35" t="s">
+        <v>269</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>265</v>
+        <v>270</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>271</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -3272,13 +3340,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -3292,13 +3360,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -3307,18 +3375,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -3327,18 +3395,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -3347,18 +3415,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -3371,14 +3439,14 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="33" t="s">
-        <v>281</v>
+      <c r="A14" s="35" t="s">
+        <v>287</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>283</v>
+        <v>288</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>289</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -3392,13 +3460,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -3412,13 +3480,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -3427,18 +3495,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -3447,18 +3515,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -3467,18 +3535,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -3492,13 +3560,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -3511,146 +3579,146 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="34" t="s">
-        <v>302</v>
-      </c>
-      <c r="B21" s="35" t="s">
+      <c r="A21" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="B21" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="34" t="s">
-        <v>303</v>
-      </c>
-      <c r="D21" s="36">
+      <c r="C21" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="D21" s="38">
         <v>44734.0</v>
       </c>
-      <c r="E21" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="37" t="s">
+      <c r="E21" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="34"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
     </row>
     <row r="22">
-      <c r="A22" s="34" t="s">
-        <v>304</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>305</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>306</v>
-      </c>
-      <c r="D22" s="36">
+      <c r="A22" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>311</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="D22" s="38">
         <v>44734.0</v>
       </c>
-      <c r="E22" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="37" t="s">
+      <c r="E22" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="34"/>
-      <c r="V22" s="34"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="36"/>
+      <c r="V22" s="36"/>
     </row>
     <row r="23">
-      <c r="A23" s="34" t="s">
-        <v>307</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>308</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>309</v>
-      </c>
-      <c r="D23" s="36">
+      <c r="A23" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>314</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="D23" s="38">
         <v>44734.0</v>
       </c>
-      <c r="E23" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="37" t="s">
+      <c r="E23" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="34"/>
-      <c r="V23" s="34"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="36"/>
+      <c r="U23" s="36"/>
+      <c r="V23" s="36"/>
     </row>
     <row r="24">
-      <c r="A24" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>311</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>312</v>
-      </c>
-      <c r="D24" s="36">
+      <c r="A24" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>318</v>
+      </c>
+      <c r="D24" s="38">
         <v>45189.0</v>
       </c>
-      <c r="E24" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="34"/>
-      <c r="V24" s="34"/>
+      <c r="E24" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="36"/>
+      <c r="U24" s="36"/>
+      <c r="V24" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds P7012 extension with RDF and HTML
- Adds P7012 extension under `2.1-dev/standards/p7012`
- Contains RDF and HTML outputs for P7012
- The status of the extension is DRAFT
- See #203

Co-authored-by: Iain Henderson <iain@jlinc.com>
Co-authored-by: Beatriz Esteves <beatriz.gc.esteves@gmail.com>

Squashed commit of the following:

commit 1d3a67854a8c657502d384a8848621ef868a9455
Author: Harshvardhan Pandit <me@harshp.com>
Date:   Sun Jan 12 21:30:33 2025 +0000

    WIP: Adds P7012 HTML

commit 47d6acb76af1b80d16d57bfbff8fb77664d4a8ca
Author: Harshvardhan Pandit <me@harshp.com>
Date:   Sun Jan 12 19:09:50 2025 +0000

    WIP: Adds P7012 RDF

commit 25b9726bedeb1e75b76b559ea5f643ab302857d0
Author: Harshvardhan Pandit <me@harshp.com>
Date:   Sun Jan 12 18:47:38 2025 +0000

    WIP: Adds P7012 CSV sources
</commit_message>
<xml_diff>
--- a/code/vocab_csv/namespaces.xlsx
+++ b/code/vocab_csv/namespaces.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="340">
   <si>
     <t>preffix</t>
   </si>
@@ -580,6 +580,15 @@
   </si>
   <si>
     <t>Public Services Sector</t>
+  </si>
+  <si>
+    <t>p7012</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/standards/p7012#</t>
+  </si>
+  <si>
+    <t>Concepts for IEEE P7012</t>
   </si>
   <si>
     <t>dct</t>
@@ -2661,6 +2670,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D62" s="23">
+        <v>45992.0</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -2725,8 +2751,9 @@
     <hyperlink r:id="rId60" ref="B59"/>
     <hyperlink r:id="rId61" ref="B60"/>
     <hyperlink r:id="rId62" ref="B61"/>
+    <hyperlink r:id="rId63" ref="B62"/>
   </hyperlinks>
-  <drawing r:id="rId63"/>
+  <drawing r:id="rId64"/>
 </worksheet>
 </file>
 
@@ -2772,13 +2799,13 @@
     </row>
     <row r="2">
       <c r="A2" s="24" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
@@ -2802,13 +2829,13 @@
     </row>
     <row r="3">
       <c r="A3" s="27" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
@@ -2832,13 +2859,13 @@
     </row>
     <row r="4">
       <c r="A4" s="27" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -2862,13 +2889,13 @@
     </row>
     <row r="5">
       <c r="A5" s="27" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
@@ -2892,13 +2919,13 @@
     </row>
     <row r="6">
       <c r="A6" s="27" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -2922,13 +2949,13 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -2952,10 +2979,10 @@
     </row>
     <row r="8">
       <c r="A8" s="24" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C8" s="30" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
@@ -2983,13 +3010,13 @@
     </row>
     <row r="9">
       <c r="A9" s="24" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
@@ -3013,13 +3040,13 @@
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -3043,13 +3070,13 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -3073,13 +3100,13 @@
     </row>
     <row r="12">
       <c r="A12" s="24" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
@@ -3103,13 +3130,13 @@
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
@@ -3133,13 +3160,13 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
@@ -3163,145 +3190,145 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3349,10 +3376,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="34" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>28</v>
@@ -3369,13 +3396,13 @@
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -3389,13 +3416,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -3409,13 +3436,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -3424,18 +3451,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -3444,34 +3471,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -3485,13 +3512,13 @@
     </row>
     <row r="8">
       <c r="A8" s="36" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -3505,13 +3532,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -3525,13 +3552,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -3540,18 +3567,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -3560,18 +3587,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -3580,18 +3607,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -3605,13 +3632,13 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -3625,13 +3652,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -3645,13 +3672,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -3660,18 +3687,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -3680,18 +3707,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -3700,18 +3727,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -3725,13 +3752,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -3745,13 +3772,13 @@
     </row>
     <row r="21">
       <c r="A21" s="37" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D21" s="39">
         <v>44734.0</v>
@@ -3781,13 +3808,13 @@
     </row>
     <row r="22">
       <c r="A22" s="37" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D22" s="39">
         <v>44734.0</v>
@@ -3817,13 +3844,13 @@
     </row>
     <row r="23">
       <c r="A23" s="37" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D23" s="39">
         <v>44734.0</v>
@@ -3853,13 +3880,13 @@
     </row>
     <row r="24">
       <c r="A24" s="37" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D24" s="39">
         <v>45189.0</v>

</xml_diff>

<commit_message>
update namespaces for legal extensions
- closes #291
- fixes typo mentioned in #292

Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/namespaces.xlsx
+++ b/code/vocab_csv/namespaces.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="373">
   <si>
     <t>preffix</t>
   </si>
@@ -526,6 +526,87 @@
   </si>
   <si>
     <t>Laws and Authorities for US</t>
+  </si>
+  <si>
+    <t>legal-hk</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/hk#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for HK</t>
+  </si>
+  <si>
+    <t>legal-jp</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/jp#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for JP</t>
+  </si>
+  <si>
+    <t>legal-kr</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/kr#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for KR</t>
+  </si>
+  <si>
+    <t>legal-mo</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/mo#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for MO</t>
+  </si>
+  <si>
+    <t>legal-my</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/my#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for MY</t>
+  </si>
+  <si>
+    <t>legal-ph</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/ph#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for PH</t>
+  </si>
+  <si>
+    <t>legal-sg</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/sg#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for SG</t>
+  </si>
+  <si>
+    <t>legal-th</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/th#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for TH</t>
+  </si>
+  <si>
+    <t>legal-tw</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/tw#</t>
+  </si>
+  <si>
+    <t>Laws and Authorities for TW</t>
   </si>
   <si>
     <t>sector-education</t>
@@ -2596,8 +2677,8 @@
       <c r="C56" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D56" s="23">
-        <v>45627.0</v>
+      <c r="D56" s="8">
+        <v>45736.0</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>11</v>
@@ -2607,14 +2688,14 @@
       <c r="A57" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>175</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="D57" s="23">
-        <v>45627.0</v>
+      <c r="D57" s="8">
+        <v>45736.0</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>11</v>
@@ -2624,14 +2705,14 @@
       <c r="A58" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>178</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D58" s="23">
-        <v>45627.0</v>
+      <c r="D58" s="8">
+        <v>45736.0</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>11</v>
@@ -2641,14 +2722,14 @@
       <c r="A59" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>181</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D59" s="23">
-        <v>45627.0</v>
+      <c r="D59" s="8">
+        <v>45736.0</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>11</v>
@@ -2658,14 +2739,14 @@
       <c r="A60" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="9" t="s">
         <v>184</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D60" s="23">
-        <v>45627.0</v>
+      <c r="D60" s="8">
+        <v>45736.0</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>11</v>
@@ -2675,14 +2756,14 @@
       <c r="A61" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="9" t="s">
         <v>187</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="D61" s="23">
-        <v>45627.0</v>
+      <c r="D61" s="8">
+        <v>45736.0</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>11</v>
@@ -2692,16 +2773,169 @@
       <c r="A62" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="9" t="s">
         <v>190</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D62" s="23">
+      <c r="D62" s="8">
+        <v>45736.0</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D63" s="8">
+        <v>45736.0</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D64" s="8">
+        <v>45736.0</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D65" s="23">
+        <v>45627.0</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D66" s="23">
+        <v>45627.0</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D67" s="23">
+        <v>45627.0</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D68" s="23">
+        <v>45627.0</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D69" s="23">
+        <v>45627.0</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D70" s="23">
+        <v>45627.0</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D71" s="23">
         <v>45992.0</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E71" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2770,8 +3004,17 @@
     <hyperlink r:id="rId61" ref="B60"/>
     <hyperlink r:id="rId62" ref="B61"/>
     <hyperlink r:id="rId63" ref="B62"/>
+    <hyperlink r:id="rId64" ref="B63"/>
+    <hyperlink r:id="rId65" ref="B64"/>
+    <hyperlink r:id="rId66" ref="B65"/>
+    <hyperlink r:id="rId67" ref="B66"/>
+    <hyperlink r:id="rId68" ref="B67"/>
+    <hyperlink r:id="rId69" ref="B68"/>
+    <hyperlink r:id="rId70" ref="B69"/>
+    <hyperlink r:id="rId71" ref="B70"/>
+    <hyperlink r:id="rId72" ref="B71"/>
   </hyperlinks>
-  <drawing r:id="rId64"/>
+  <drawing r:id="rId73"/>
 </worksheet>
 </file>
 
@@ -2817,13 +3060,13 @@
     </row>
     <row r="2">
       <c r="A2" s="24" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
@@ -2847,13 +3090,13 @@
     </row>
     <row r="3">
       <c r="A3" s="27" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
@@ -2877,13 +3120,13 @@
     </row>
     <row r="4">
       <c r="A4" s="27" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -2907,13 +3150,13 @@
     </row>
     <row r="5">
       <c r="A5" s="27" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
@@ -2937,13 +3180,13 @@
     </row>
     <row r="6">
       <c r="A6" s="27" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -2967,13 +3210,13 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -2997,10 +3240,10 @@
     </row>
     <row r="8">
       <c r="A8" s="24" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
       <c r="C8" s="30" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
@@ -3028,13 +3271,13 @@
     </row>
     <row r="9">
       <c r="A9" s="24" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
@@ -3058,13 +3301,13 @@
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>217</v>
+        <v>244</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -3088,13 +3331,13 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>218</v>
+        <v>245</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>219</v>
+        <v>246</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -3118,13 +3361,13 @@
     </row>
     <row r="12">
       <c r="A12" s="24" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>222</v>
+        <v>249</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>223</v>
+        <v>250</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
@@ -3148,13 +3391,13 @@
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
@@ -3178,13 +3421,13 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>227</v>
+        <v>254</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>228</v>
+        <v>255</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
@@ -3208,167 +3451,167 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>232</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>262</v>
+        <v>289</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>263</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>264</v>
+        <v>291</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>266</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>267</v>
+        <v>294</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>270</v>
+        <v>297</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>272</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3418,10 +3661,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="34" t="s">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>28</v>
@@ -3438,13 +3681,13 @@
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>275</v>
+        <v>302</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>276</v>
+        <v>303</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -3458,13 +3701,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -3478,13 +3721,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>283</v>
+        <v>310</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -3493,18 +3736,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>284</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>285</v>
+        <v>312</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>287</v>
+        <v>314</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -3513,34 +3756,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>289</v>
+        <v>316</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>290</v>
+        <v>317</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>291</v>
+        <v>318</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>292</v>
+        <v>319</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>293</v>
+        <v>320</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>294</v>
+        <v>321</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -3554,13 +3797,13 @@
     </row>
     <row r="8">
       <c r="A8" s="36" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>297</v>
+        <v>324</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -3574,13 +3817,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>299</v>
+        <v>326</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>301</v>
+        <v>328</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -3594,13 +3837,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>302</v>
+        <v>329</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>304</v>
+        <v>331</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -3609,18 +3852,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>284</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -3629,18 +3872,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>309</v>
+        <v>336</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>310</v>
+        <v>337</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -3649,18 +3892,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>312</v>
+        <v>339</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>313</v>
+        <v>340</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -3674,13 +3917,13 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>314</v>
+        <v>341</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>315</v>
+        <v>342</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>316</v>
+        <v>343</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -3694,13 +3937,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>317</v>
+        <v>344</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>318</v>
+        <v>345</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>319</v>
+        <v>346</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -3714,13 +3957,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>320</v>
+        <v>347</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>322</v>
+        <v>349</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -3729,18 +3972,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>284</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>323</v>
+        <v>350</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>324</v>
+        <v>351</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>325</v>
+        <v>352</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -3749,18 +3992,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>326</v>
+        <v>353</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>327</v>
+        <v>354</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>328</v>
+        <v>355</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -3769,18 +4012,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>329</v>
+        <v>356</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>331</v>
+        <v>358</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -3794,13 +4037,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>332</v>
+        <v>359</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>333</v>
+        <v>360</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>334</v>
+        <v>361</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -3814,13 +4057,13 @@
     </row>
     <row r="21">
       <c r="A21" s="37" t="s">
-        <v>335</v>
+        <v>362</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>336</v>
+        <v>363</v>
       </c>
       <c r="D21" s="39">
         <v>44734.0</v>
@@ -3850,13 +4093,13 @@
     </row>
     <row r="22">
       <c r="A22" s="37" t="s">
-        <v>337</v>
+        <v>364</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>338</v>
+        <v>365</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>339</v>
+        <v>366</v>
       </c>
       <c r="D22" s="39">
         <v>44734.0</v>
@@ -3886,13 +4129,13 @@
     </row>
     <row r="23">
       <c r="A23" s="37" t="s">
-        <v>340</v>
+        <v>367</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>341</v>
+        <v>368</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>342</v>
+        <v>369</v>
       </c>
       <c r="D23" s="39">
         <v>44734.0</v>
@@ -3922,13 +4165,13 @@
     </row>
     <row r="24">
       <c r="A24" s="37" t="s">
-        <v>343</v>
+        <v>370</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>344</v>
+        <v>371</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>345</v>
+        <v>372</v>
       </c>
       <c r="D24" s="39">
         <v>45189.0</v>

</xml_diff>

<commit_message>
Change P7012 to IEEE-7012 ; extend DPV concepts
- changed "P7012" title and structure to "IEEE 7012"; see #423
- P7012 was the draft number, the published number is just 7012
- changed title, namespace, filenames (CSV, RDF, HTML)
- folder structure is now `standards/ieee/7012` (breaks urls)
- NOTE: REQUIRES UPDATE TO W3ID ; use #425
- downloaded CSV files with new name, regenerated RDF and HTML
- updated index
- 7012 concepts for purpose now extend the DPV concepts
- TODO: update Agent concepts once added to DPV

Co-authored-by: Iain Henderson <iain@jlinc.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/namespaces.xlsx
+++ b/code/vocab_csv/namespaces.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Namespaces" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Namespaces_Other" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Namespaces_old" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Namespaces" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Namespaces_Other" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Namespaces_old" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="378">
   <si>
     <t>prefix</t>
   </si>
@@ -663,13 +663,28 @@
     <t>Public Services Sector</t>
   </si>
   <si>
-    <t>p7012</t>
-  </si>
-  <si>
-    <t>https://w3id.org/dpv/standards/p7012#</t>
-  </si>
-  <si>
-    <t>Concepts for IEEE P7012</t>
+    <t>ieee-7012</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/standards/ieee/7012#</t>
+  </si>
+  <si>
+    <t>Concepts for IEEE 7012</t>
+  </si>
+  <si>
+    <t>modified</t>
+  </si>
+  <si>
+    <t>de-gdng</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/de/gdng#</t>
+  </si>
+  <si>
+    <t>GDNG (DE) concepts extending DPV</t>
+  </si>
+  <si>
+    <t>28/01/2026</t>
   </si>
   <si>
     <t>dct</t>
@@ -1473,6 +1488,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
@@ -2933,9 +2952,26 @@
         <v>218</v>
       </c>
       <c r="D71" s="23">
-        <v>45992.0</v>
+        <v>46055.0</v>
       </c>
       <c r="E71" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3013,8 +3049,9 @@
     <hyperlink r:id="rId70" ref="B69"/>
     <hyperlink r:id="rId71" ref="B70"/>
     <hyperlink r:id="rId72" ref="B71"/>
+    <hyperlink r:id="rId73" ref="B72"/>
   </hyperlinks>
-  <drawing r:id="rId73"/>
+  <drawing r:id="rId74"/>
 </worksheet>
 </file>
 
@@ -3060,13 +3097,13 @@
     </row>
     <row r="2">
       <c r="A2" s="24" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
@@ -3090,13 +3127,13 @@
     </row>
     <row r="3">
       <c r="A3" s="27" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
@@ -3120,13 +3157,13 @@
     </row>
     <row r="4">
       <c r="A4" s="27" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -3150,13 +3187,13 @@
     </row>
     <row r="5">
       <c r="A5" s="27" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
@@ -3180,13 +3217,13 @@
     </row>
     <row r="6">
       <c r="A6" s="27" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -3210,13 +3247,13 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -3240,10 +3277,10 @@
     </row>
     <row r="8">
       <c r="A8" s="24" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C8" s="30" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
@@ -3271,13 +3308,13 @@
     </row>
     <row r="9">
       <c r="A9" s="24" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
@@ -3301,13 +3338,13 @@
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -3331,13 +3368,13 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -3361,13 +3398,13 @@
     </row>
     <row r="12">
       <c r="A12" s="24" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
@@ -3391,13 +3428,13 @@
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
@@ -3421,13 +3458,13 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
@@ -3451,167 +3488,167 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3661,10 +3698,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="34" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>28</v>
@@ -3681,13 +3718,13 @@
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -3701,13 +3738,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -3721,13 +3758,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -3736,18 +3773,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -3756,34 +3793,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -3797,13 +3834,13 @@
     </row>
     <row r="8">
       <c r="A8" s="36" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -3817,13 +3854,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -3837,13 +3874,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -3852,18 +3889,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -3872,18 +3909,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -3892,18 +3929,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -3917,13 +3954,13 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -3937,13 +3974,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -3957,13 +3994,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -3972,18 +4009,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -3992,18 +4029,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -4012,18 +4049,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -4037,13 +4074,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -4057,13 +4094,13 @@
     </row>
     <row r="21">
       <c r="A21" s="37" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="D21" s="39">
         <v>44734.0</v>
@@ -4093,13 +4130,13 @@
     </row>
     <row r="22">
       <c r="A22" s="37" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="D22" s="39">
         <v>44734.0</v>
@@ -4129,13 +4166,13 @@
     </row>
     <row r="23">
       <c r="A23" s="37" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="D23" s="39">
         <v>44734.0</v>
@@ -4165,13 +4202,13 @@
     </row>
     <row r="24">
       <c r="A24" s="37" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="D24" s="39">
         <v>45189.0</v>

</xml_diff>

<commit_message>
create IN-DPDP extension #438
- creates `/legal/in/dpdp` extension
- adds folder structure, metadata in `vocab_management.py`, template for
  HTML as `template_legal_in_dpdp`, and namespace as `in-dpdp`
- includes RDF and HTML outputs with lawfulness/compliance concepts

Co-authored-by: Ajay Jadhav <ajay@ayanworks.com>
(cherry picked from commit 868febda49833633aee988e5a38d2cb9ceee784d)
</commit_message>
<xml_diff>
--- a/code/vocab_csv/namespaces.xlsx
+++ b/code/vocab_csv/namespaces.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="382">
   <si>
     <t>prefix</t>
   </si>
@@ -685,6 +685,18 @@
   </si>
   <si>
     <t>28/01/2026</t>
+  </si>
+  <si>
+    <t>in-dpdp</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/in/dpdp#</t>
+  </si>
+  <si>
+    <t>DPDP (IN) concepts extending DPV</t>
+  </si>
+  <si>
+    <t>22/02/2026</t>
   </si>
   <si>
     <t>dct</t>
@@ -2975,6 +2987,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -3050,8 +3079,9 @@
     <hyperlink r:id="rId71" ref="B70"/>
     <hyperlink r:id="rId72" ref="B71"/>
     <hyperlink r:id="rId73" ref="B72"/>
+    <hyperlink r:id="rId74" ref="B73"/>
   </hyperlinks>
-  <drawing r:id="rId74"/>
+  <drawing r:id="rId75"/>
 </worksheet>
 </file>
 
@@ -3097,13 +3127,13 @@
     </row>
     <row r="2">
       <c r="A2" s="24" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
@@ -3127,13 +3157,13 @@
     </row>
     <row r="3">
       <c r="A3" s="27" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
@@ -3157,13 +3187,13 @@
     </row>
     <row r="4">
       <c r="A4" s="27" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -3187,13 +3217,13 @@
     </row>
     <row r="5">
       <c r="A5" s="27" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
@@ -3217,13 +3247,13 @@
     </row>
     <row r="6">
       <c r="A6" s="27" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -3247,13 +3277,13 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -3277,10 +3307,10 @@
     </row>
     <row r="8">
       <c r="A8" s="24" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C8" s="30" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
@@ -3308,13 +3338,13 @@
     </row>
     <row r="9">
       <c r="A9" s="24" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
@@ -3338,13 +3368,13 @@
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -3368,13 +3398,13 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -3398,13 +3428,13 @@
     </row>
     <row r="12">
       <c r="A12" s="24" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
@@ -3428,13 +3458,13 @@
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
@@ -3458,13 +3488,13 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
@@ -3488,167 +3518,167 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3698,10 +3728,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="34" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>28</v>
@@ -3718,13 +3748,13 @@
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -3738,13 +3768,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -3758,13 +3788,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -3773,18 +3803,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -3793,34 +3823,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -3834,13 +3864,13 @@
     </row>
     <row r="8">
       <c r="A8" s="36" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -3854,13 +3884,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -3874,13 +3904,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -3889,18 +3919,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -3909,18 +3939,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -3929,18 +3959,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -3954,13 +3984,13 @@
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -3974,13 +4004,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -3994,13 +4024,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -4009,18 +4039,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -4029,18 +4059,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -4049,18 +4079,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -4074,13 +4104,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -4094,13 +4124,13 @@
     </row>
     <row r="21">
       <c r="A21" s="37" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D21" s="39">
         <v>44734.0</v>
@@ -4130,13 +4160,13 @@
     </row>
     <row r="22">
       <c r="A22" s="37" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D22" s="39">
         <v>44734.0</v>
@@ -4166,13 +4196,13 @@
     </row>
     <row r="23">
       <c r="A23" s="37" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D23" s="39">
         <v>44734.0</v>
@@ -4202,13 +4232,13 @@
     </row>
     <row r="24">
       <c r="A24" s="37" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D24" s="39">
         <v>45189.0</v>

</xml_diff>